<commit_message>
RequirementData 시트 이름 수정
</commit_message>
<xml_diff>
--- a/excel/RequirementData.xlsx
+++ b/excel/RequirementData.xlsx
@@ -5,15 +5,15 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/geugkkom/Documents/Tsomsomm/sp-data/excel/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/geugkkom/Documents/Tsomsomm/lunaria-data/excel/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3573C4EF-29F4-E546-BB5E-F742C236DDDB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6BDE33E-390B-F644-BF1D-1C4F4BAAFF38}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="7000" yWindow="5080" windowWidth="21600" windowHeight="11300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="RequirementInfo" sheetId="1" r:id="rId1"/>
+    <sheet name="RequirementInfoData" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
@@ -481,7 +481,7 @@
   <dimension ref="A1:F12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>

</xml_diff>